<commit_message>
Cmbios datos excel, Se agregaron capturas, Se monitoriaron errores en gestion Facturacion, otros
</commit_message>
<xml_diff>
--- a/Datos/Datos.xlsx
+++ b/Datos/Datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Narveider\Downloads\RobotOptimus (1)\RobotOptimus\cl.bcs.optimus\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rnunez_ext\git\SeleniumRobot\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="43">
   <si>
     <t>rut</t>
   </si>
@@ -113,12 +113,6 @@
     <t>785,47</t>
   </si>
   <si>
-    <t>690,56</t>
-  </si>
-  <si>
-    <t>695,56</t>
-  </si>
-  <si>
     <t>1,1041</t>
   </si>
   <si>
@@ -156,6 +150,9 @@
   </si>
   <si>
     <t>operacion</t>
+  </si>
+  <si>
+    <t>640,56</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="I6" activeCellId="2" sqref="I3 I7 I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,12 +531,12 @@
         <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -563,7 +560,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>18</v>
@@ -575,12 +572,12 @@
         <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -604,7 +601,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
@@ -616,12 +613,12 @@
         <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -654,15 +651,15 @@
         <v>20</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -695,15 +692,15 @@
         <v>20</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -727,7 +724,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>18</v>
@@ -739,12 +736,12 @@
         <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -768,7 +765,7 @@
         <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
@@ -780,12 +777,12 @@
         <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -818,15 +815,15 @@
         <v>20</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -859,15 +856,15 @@
         <v>20</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -903,12 +900,12 @@
         <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -944,12 +941,12 @@
         <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -985,12 +982,12 @@
         <v>5</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -1026,7 +1023,7 @@
         <v>5</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>